<commit_message>
Update Average vector method Alcohol Dehydration.ipynb
</commit_message>
<xml_diff>
--- a/database/Alcohol_Dyhydration.xlsx
+++ b/database/Alcohol_Dyhydration.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>Reactants</t>
   </si>
@@ -79,6 +79,38 @@
   </si>
   <si>
     <t>CCCOC(C)C</t>
+  </si>
+  <si>
+    <t>Ethanol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Propanol</t>
+  </si>
+  <si>
+    <t>Butanol</t>
+  </si>
+  <si>
+    <t>Isopropanol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Isobutanol</t>
+  </si>
+  <si>
+    <t>OCC(C)C</t>
+  </si>
+  <si>
+    <t>COCC(C)C</t>
+  </si>
+  <si>
+    <t>CCOCC(C)C</t>
+  </si>
+  <si>
+    <t>CCCOCC(C)C</t>
+  </si>
+  <si>
+    <t>CC(OCC(C)C)C</t>
   </si>
 </sst>
 </file>
@@ -121,10 +153,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,120 +441,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D14" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>